<commit_message>
Project Cleanup and added some missing translations
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4CF9FE-42DF-4EB8-9E2A-54B98432F101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B6CA12-2057-40A8-92BD-3CD179199BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8964" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>Polish</t>
   </si>
@@ -108,6 +108,42 @@
   </si>
   <si>
     <t>Lose 1 time</t>
+  </si>
+  <si>
+    <t>MUSIC</t>
+  </si>
+  <si>
+    <t>SOUND</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>LEVELS</t>
+  </si>
+  <si>
+    <t>Muzyka</t>
+  </si>
+  <si>
+    <t>Dźwięk</t>
+  </si>
+  <si>
+    <t>Język</t>
+  </si>
+  <si>
+    <t>Poziomy</t>
+  </si>
+  <si>
+    <t>Levels</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Music</t>
   </si>
 </sst>
 </file>
@@ -470,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,23 +599,67 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added loading screen and new gamemodes
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B6CA12-2057-40A8-92BD-3CD179199BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA52E5D-C219-4CB3-913D-5117BBE690F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
   <si>
     <t>Polish</t>
   </si>
@@ -144,6 +144,171 @@
   </si>
   <si>
     <t>Music</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>REMEMBER</t>
+  </si>
+  <si>
+    <t>LOGIN</t>
+  </si>
+  <si>
+    <t>REGISTERANDLOGIN</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>SEARCH</t>
+  </si>
+  <si>
+    <t>EASY</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>HARD</t>
+  </si>
+  <si>
+    <t>QUESTION</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>CORRECTANSWER</t>
+  </si>
+  <si>
+    <t>INCORRECTANSWER</t>
+  </si>
+  <si>
+    <t>TIMEISUP</t>
+  </si>
+  <si>
+    <t>PLAYAGAIN</t>
+  </si>
+  <si>
+    <t>REMAININGTIME</t>
+  </si>
+  <si>
+    <t>SCORE</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Hasło</t>
+  </si>
+  <si>
+    <t>Zapamiętaj</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Zarejestruj i zaloguj</t>
+  </si>
+  <si>
+    <t>Powrót</t>
+  </si>
+  <si>
+    <t>Wynik</t>
+  </si>
+  <si>
+    <t>Łatwy</t>
+  </si>
+  <si>
+    <t>Średni</t>
+  </si>
+  <si>
+    <t>Trudny</t>
+  </si>
+  <si>
+    <t>Pytanie</t>
+  </si>
+  <si>
+    <t>Czas</t>
+  </si>
+  <si>
+    <t>Poprawne odpowiedzi</t>
+  </si>
+  <si>
+    <t>Niepoprawne odpowiedzi</t>
+  </si>
+  <si>
+    <t>Czas minał</t>
+  </si>
+  <si>
+    <t>Zagraj jeszcze raz</t>
+  </si>
+  <si>
+    <t>Pozostały czas</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Remember</t>
+  </si>
+  <si>
+    <t>Return</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Hard</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Register and login</t>
+  </si>
+  <si>
+    <t>Correct answers</t>
+  </si>
+  <si>
+    <t>Incorrect answers</t>
+  </si>
+  <si>
+    <t>Time is up</t>
+  </si>
+  <si>
+    <t>Play again</t>
+  </si>
+  <si>
+    <t>Remaining time</t>
+  </si>
+  <si>
+    <t>Szukaj…</t>
+  </si>
+  <si>
+    <t>Search…</t>
+  </si>
+  <si>
+    <t>NICKNAME</t>
+  </si>
+  <si>
+    <t>Nazwa</t>
+  </si>
+  <si>
+    <t>Nickname</t>
   </si>
 </sst>
 </file>
@@ -506,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,23 +808,232 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B32" t="s">
         <v>22</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C32" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new achievements and translations
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA71B1C1-1D55-4A76-AB67-D6F8A1C888A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5F1D3B19-8459-4E15-8262-89380ECFEDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Translations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="121">
   <si>
     <t>Polish</t>
   </si>
@@ -345,6 +345,60 @@
   </si>
   <si>
     <t>Answer 200 questions</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>CONFIRM</t>
+  </si>
+  <si>
+    <t>Wskaż</t>
+  </si>
+  <si>
+    <t>Potwierdź</t>
+  </si>
+  <si>
+    <t>SOLVEQUIZUNDER120</t>
+  </si>
+  <si>
+    <t>SOLVEQUIZUNDER60</t>
+  </si>
+  <si>
+    <t>SOLVEQUIZUNDER30</t>
+  </si>
+  <si>
+    <t>Rozwiąż dowolny quiz w mniej niż 2 minuty</t>
+  </si>
+  <si>
+    <t>Rozwiąż dowolny quiz w mniej niż 30 sekund</t>
+  </si>
+  <si>
+    <t>Rozwiąż dowolny quiz w mniej niż 1 minutę</t>
+  </si>
+  <si>
+    <t>Solve any quiz under 2 minutes</t>
+  </si>
+  <si>
+    <t>Solve any quiz under 1 minute</t>
+  </si>
+  <si>
+    <t>Solve any quiz under 30 seconds</t>
+  </si>
+  <si>
+    <t>SOLVEQUIZUNDERLAST5</t>
+  </si>
+  <si>
+    <t>Rozwiąż dowolny quiz w ostanich 5 sekundach</t>
+  </si>
+  <si>
+    <t>Solve any quiz in last 5 seconds</t>
   </si>
 </sst>
 </file>
@@ -707,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1052,68 +1106,134 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="C34" t="s">
-        <v>94</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>90</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>98</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Flexible element searching, confetti particle system, new translaitons, refresh leaderboard button
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5F1D3B19-8459-4E15-8262-89380ECFEDAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1768A1-1B9F-43CB-90A3-F003C802C669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="124">
   <si>
     <t>Polish</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>Solve any quiz in last 5 seconds</t>
+  </si>
+  <si>
+    <t>REFRESH</t>
+  </si>
+  <si>
+    <t>Odśwież</t>
+  </si>
+  <si>
+    <t>Refresh</t>
   </si>
 </sst>
 </file>
@@ -761,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1128,111 +1137,122 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>118</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>119</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new sound, conffeti particles and some UI elements
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1768A1-1B9F-43CB-90A3-F003C802C669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FD2701-A0E2-44C0-85D4-8876DE18041C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="127">
   <si>
     <t>Polish</t>
   </si>
@@ -408,6 +408,15 @@
   </si>
   <si>
     <t>Refresh</t>
+  </si>
+  <si>
+    <t>COMPLETED</t>
+  </si>
+  <si>
+    <t>Zdobyte:</t>
+  </si>
+  <si>
+    <t>Completed:</t>
   </si>
 </sst>
 </file>
@@ -770,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1148,111 +1157,122 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>102</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B37" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C37" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>118</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>119</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Handle missing translation, added elements types
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F4FD3D-2AFE-4617-82DC-A021C3F5BEFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{573F778B-6E6F-4CFC-87D6-B052E19370E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="192">
   <si>
     <t>Polish</t>
   </si>
@@ -440,15 +440,6 @@
     <t>Łąkotka przyśrodkowa</t>
   </si>
   <si>
-    <t>Staw piszczelowy</t>
-  </si>
-  <si>
-    <t>Staw rzepkowy</t>
-  </si>
-  <si>
-    <t>Staw strzałkowy</t>
-  </si>
-  <si>
     <t>Więzadło poprzeczne</t>
   </si>
   <si>
@@ -479,12 +470,6 @@
     <t>Patella</t>
   </si>
   <si>
-    <t>Lateral collateral ligaments</t>
-  </si>
-  <si>
-    <t>Medial collateral ligaments</t>
-  </si>
-  <si>
     <t>Lateral meniscus</t>
   </si>
   <si>
@@ -500,15 +485,9 @@
     <t>Posterior cruciate ligament</t>
   </si>
   <si>
-    <t>The posterior meniscus-femoral ligament</t>
-  </si>
-  <si>
     <t>Patellar ligament</t>
   </si>
   <si>
-    <t>Sagittal joint</t>
-  </si>
-  <si>
     <t>Patella joint</t>
   </si>
   <si>
@@ -527,40 +506,112 @@
     <t>PATELLA</t>
   </si>
   <si>
-    <t>MEDIAL CONDYLE</t>
-  </si>
-  <si>
-    <t>LATERAL MENISCUS</t>
-  </si>
-  <si>
-    <t>MEDIAL MENISCUS</t>
-  </si>
-  <si>
-    <t>TIBIAL JOINT</t>
-  </si>
-  <si>
-    <t>PATELLA JOINT</t>
-  </si>
-  <si>
-    <t>SAGITTAL JOINT</t>
-  </si>
-  <si>
-    <t>TRANSVERSE LIGAMENT</t>
-  </si>
-  <si>
-    <t>POSTERIOR CRUCIATE LIGAMENT</t>
-  </si>
-  <si>
-    <t>THE POSTERIOR MENISCUS-FEMORAL LIGAMENT</t>
-  </si>
-  <si>
-    <t>MEDIAL COLLATERAL LIGAMENTS</t>
-  </si>
-  <si>
-    <t>LATERAL COLLATERAL LIGAMENTS</t>
-  </si>
-  <si>
-    <t>PATELLAR LIGAMENT</t>
+    <t>Latin</t>
+  </si>
+  <si>
+    <t>Ligamentum cruciatum posterius</t>
+  </si>
+  <si>
+    <t>Ligamentum transversum genus</t>
+  </si>
+  <si>
+    <t>Posterior meniscofemoral ligament</t>
+  </si>
+  <si>
+    <t>Ligamentum meniscofemorale posterius</t>
+  </si>
+  <si>
+    <t>Meniscus medialis</t>
+  </si>
+  <si>
+    <t>Meniscus lateralis</t>
+  </si>
+  <si>
+    <t>Ligamentum collaterale fibulare genus</t>
+  </si>
+  <si>
+    <t>Ligamentum patellae</t>
+  </si>
+  <si>
+    <t>Condylus medialis femoris</t>
+  </si>
+  <si>
+    <t>Tibial collateral ligament</t>
+  </si>
+  <si>
+    <t>Fibular collateral ligament</t>
+  </si>
+  <si>
+    <t>Ligamentum collaterale tibiale genus</t>
+  </si>
+  <si>
+    <t>Powierzchnia stawowa strzałki</t>
+  </si>
+  <si>
+    <t>Articular facet of head of fibula</t>
+  </si>
+  <si>
+    <t>Facies articularis capitis fibulae</t>
+  </si>
+  <si>
+    <t>Powierzchnia stawowa piszczela</t>
+  </si>
+  <si>
+    <t>Powierzchnia stawowa rzepki</t>
+  </si>
+  <si>
+    <t>Os femoris</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>TIBIALJOINT</t>
+  </si>
+  <si>
+    <t>PATELLAJOINT</t>
+  </si>
+  <si>
+    <t>SAGITTALJOINT</t>
+  </si>
+  <si>
+    <t>TRANSVERSELIGAMENT</t>
+  </si>
+  <si>
+    <t>POSTERIORCRUCIATELIGAMENT</t>
+  </si>
+  <si>
+    <t>POSTERIORMENISCUS-FEMORALLIGAMENT</t>
+  </si>
+  <si>
+    <t>MEDIALCOLLATERALLIGAMENTS</t>
+  </si>
+  <si>
+    <t>LATERALCOLLATERALLIGAMENTS</t>
+  </si>
+  <si>
+    <t>PATELLARLIGAMENT</t>
+  </si>
+  <si>
+    <t>LATERALMENISCUS</t>
+  </si>
+  <si>
+    <t>MEDIALMENISCUS</t>
+  </si>
+  <si>
+    <t>MEDIALCONDYLE</t>
+  </si>
+  <si>
+    <t>ANTERIORCRUCIATELIGAMNET</t>
+  </si>
+  <si>
+    <t>Więzadło krzyżowe przednie</t>
+  </si>
+  <si>
+    <t>Anterior cruciate ligament</t>
+  </si>
+  <si>
+    <t>Ligamentum cruciatum anterius</t>
   </si>
 </sst>
 </file>
@@ -606,9 +657,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -923,16 +975,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -945,10 +998,12 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -957,9 +1012,12 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -968,9 +1026,12 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
+      <c r="D3" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
@@ -979,9 +1040,12 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
+      <c r="D4" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
@@ -990,9 +1054,12 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
+      <c r="D5" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -1001,9 +1068,12 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
+      <c r="D6" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
@@ -1012,9 +1082,12 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
+      <c r="D7" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" t="s">
@@ -1023,9 +1096,12 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
+      <c r="D8" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
@@ -1034,9 +1110,12 @@
       <c r="C9" t="s">
         <v>31</v>
       </c>
+      <c r="D9" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" t="s">
@@ -1045,9 +1124,12 @@
       <c r="C10" t="s">
         <v>30</v>
       </c>
+      <c r="D10" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B11" t="s">
@@ -1056,9 +1138,12 @@
       <c r="C11" t="s">
         <v>29</v>
       </c>
+      <c r="D11" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
@@ -1067,9 +1152,12 @@
       <c r="C12" t="s">
         <v>51</v>
       </c>
+      <c r="D12" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
@@ -1078,9 +1166,12 @@
       <c r="C13" t="s">
         <v>68</v>
       </c>
+      <c r="D13" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B14" t="s">
@@ -1089,9 +1180,12 @@
       <c r="C14" t="s">
         <v>87</v>
       </c>
+      <c r="D14" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B15" t="s">
@@ -1100,9 +1194,12 @@
       <c r="C15" t="s">
         <v>69</v>
       </c>
+      <c r="D15" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B16" t="s">
@@ -1111,9 +1208,12 @@
       <c r="C16" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B17" t="s">
@@ -1122,9 +1222,12 @@
       <c r="C17" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B18" t="s">
@@ -1133,9 +1236,12 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="D18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B19" t="s">
@@ -1144,9 +1250,12 @@
       <c r="C19" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D19" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B20" t="s">
@@ -1155,9 +1264,12 @@
       <c r="C20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D20" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" t="s">
@@ -1166,9 +1278,12 @@
       <c r="C21" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
@@ -1177,9 +1292,12 @@
       <c r="C22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D22" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B23" t="s">
@@ -1188,9 +1306,12 @@
       <c r="C23" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B24" t="s">
@@ -1199,9 +1320,12 @@
       <c r="C24" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B25" t="s">
@@ -1210,9 +1334,12 @@
       <c r="C25" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D25" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B26" t="s">
@@ -1221,9 +1348,12 @@
       <c r="C26" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="D26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B27" t="s">
@@ -1232,9 +1362,12 @@
       <c r="C27" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="D27" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B28" t="s">
@@ -1243,9 +1376,12 @@
       <c r="C28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="D28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B29" t="s">
@@ -1254,9 +1390,12 @@
       <c r="C29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="D29" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B30" t="s">
@@ -1265,9 +1404,12 @@
       <c r="C30" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="D30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B31" t="s">
@@ -1276,9 +1418,12 @@
       <c r="C31" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="D31" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B32" t="s">
@@ -1287,9 +1432,12 @@
       <c r="C32" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="D32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B33" t="s">
@@ -1298,9 +1446,12 @@
       <c r="C33" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="D33" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B34" t="s">
@@ -1309,9 +1460,12 @@
       <c r="C34" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="D34" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B35" t="s">
@@ -1320,9 +1474,12 @@
       <c r="C35" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="D35" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B36" t="s">
@@ -1331,9 +1488,12 @@
       <c r="C36" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="D36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B37" t="s">
@@ -1342,9 +1502,12 @@
       <c r="C37" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="D37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B38" t="s">
@@ -1353,9 +1516,12 @@
       <c r="C38" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+      <c r="D38" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B39" t="s">
@@ -1364,9 +1530,12 @@
       <c r="C39" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+      <c r="D39" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B40" t="s">
@@ -1375,9 +1544,12 @@
       <c r="C40" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="D40" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B41" t="s">
@@ -1386,9 +1558,12 @@
       <c r="C41" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+      <c r="D41" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B42" t="s">
@@ -1397,9 +1572,12 @@
       <c r="C42" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+      <c r="D42" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B43" t="s">
@@ -1408,9 +1586,12 @@
       <c r="C43" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="D43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B44" t="s">
@@ -1419,181 +1600,246 @@
       <c r="C44" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>159</v>
+      <c r="D44" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>152</v>
       </c>
       <c r="B45" t="s">
         <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>160</v>
+        <v>142</v>
+      </c>
+      <c r="D45" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="B46" t="s">
         <v>128</v>
       </c>
       <c r="C46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>161</v>
+        <v>141</v>
+      </c>
+      <c r="D46" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="B47" t="s">
         <v>129</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>162</v>
+        <v>140</v>
+      </c>
+      <c r="D47" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>155</v>
       </c>
       <c r="B48" t="s">
         <v>130</v>
       </c>
       <c r="C48" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>163</v>
+        <v>143</v>
+      </c>
+      <c r="D48" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="B49" t="s">
         <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>164</v>
+        <v>145</v>
+      </c>
+      <c r="D49" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="B50" t="s">
         <v>132</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>165</v>
+        <v>144</v>
+      </c>
+      <c r="D50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B51" t="s">
         <v>133</v>
       </c>
       <c r="C51" t="s">
+        <v>146</v>
+      </c>
+      <c r="D51" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" t="s">
+        <v>172</v>
+      </c>
+      <c r="C52" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+      <c r="D52" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B53" t="s">
+        <v>173</v>
+      </c>
+      <c r="C53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" t="s">
+        <v>169</v>
+      </c>
+      <c r="C54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B55" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" t="s">
+        <v>148</v>
+      </c>
+      <c r="D57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" t="s">
+        <v>136</v>
+      </c>
+      <c r="C58" t="s">
+        <v>159</v>
+      </c>
+      <c r="D58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B59" t="s">
+        <v>137</v>
+      </c>
+      <c r="C59" t="s">
         <v>166</v>
       </c>
-      <c r="B52" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="D59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+      <c r="C60" t="s">
         <v>167</v>
       </c>
-      <c r="B53" t="s">
-        <v>135</v>
-      </c>
-      <c r="C53" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>168</v>
-      </c>
-      <c r="B54" t="s">
-        <v>136</v>
-      </c>
-      <c r="C54" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>169</v>
-      </c>
-      <c r="B55" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>170</v>
-      </c>
-      <c r="B56" t="s">
-        <v>138</v>
-      </c>
-      <c r="C56" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>171</v>
-      </c>
-      <c r="B57" t="s">
+      <c r="D60" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B61" t="s">
         <v>139</v>
       </c>
-      <c r="C57" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>172</v>
-      </c>
-      <c r="B58" t="s">
-        <v>140</v>
-      </c>
-      <c r="C58" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" t="s">
-        <v>141</v>
-      </c>
-      <c r="C59" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>174</v>
-      </c>
-      <c r="B60" t="s">
-        <v>142</v>
-      </c>
-      <c r="C60" t="s">
-        <v>155</v>
+      <c r="C61" t="s">
+        <v>149</v>
+      </c>
+      <c r="D61" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added login information, and normalized  back button
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{26A7246D-E7DF-4B0C-8572-F56549DA3F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040C2D19-F522-4CAA-AACA-45783EA69C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="229">
   <si>
     <t>Polish</t>
   </si>
@@ -488,12 +488,6 @@
     <t>Patellar ligament</t>
   </si>
   <si>
-    <t>Patella joint</t>
-  </si>
-  <si>
-    <t>Tibial joint</t>
-  </si>
-  <si>
     <t>TIBIA</t>
   </si>
   <si>
@@ -563,9 +557,6 @@
     <t>Os femoris</t>
   </si>
   <si>
-    <t>TODO</t>
-  </si>
-  <si>
     <t>TIBIALJOINT</t>
   </si>
   <si>
@@ -695,9 +686,6 @@
     <t>What is the name of the selected item?</t>
   </si>
   <si>
-    <t>PRESSENTERTOCONFIRM</t>
-  </si>
-  <si>
     <t>Naciśnij ENTER, aby potwierdzić</t>
   </si>
   <si>
@@ -711,6 +699,30 @@
   </si>
   <si>
     <t>The email address is used</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRESSENTERTOCONFIRM </t>
+  </si>
+  <si>
+    <t>Articular surface of the tibia</t>
+  </si>
+  <si>
+    <t>Articular surface of the patella</t>
+  </si>
+  <si>
+    <t>Patellae superficies articularis</t>
+  </si>
+  <si>
+    <t>Articularis superficies tibiae</t>
+  </si>
+  <si>
+    <t>REGISTERSUCESSFUL</t>
+  </si>
+  <si>
+    <t>Zarejestrowano pomyślnie!</t>
+  </si>
+  <si>
+    <t>Register sucessful!</t>
   </si>
 </sst>
 </file>
@@ -1073,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" workbookViewId="0">
-      <selection activeCell="B62" sqref="B61:B62"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1097,10 +1109,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1113,12 +1125,6 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1130,12 +1136,6 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1147,12 +1147,6 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E4" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -1164,12 +1158,6 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -1181,12 +1169,6 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>175</v>
-      </c>
-      <c r="E6" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -1198,12 +1180,6 @@
       <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
-        <v>175</v>
-      </c>
-      <c r="E7" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -1215,12 +1191,6 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D8" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
@@ -1232,12 +1202,6 @@
       <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="D9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1249,12 +1213,6 @@
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
-        <v>175</v>
-      </c>
-      <c r="E10" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1266,12 +1224,6 @@
       <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="D11" t="s">
-        <v>175</v>
-      </c>
-      <c r="E11" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1283,12 +1235,6 @@
       <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="D12" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1300,12 +1246,6 @@
       <c r="C13" t="s">
         <v>68</v>
       </c>
-      <c r="D13" t="s">
-        <v>175</v>
-      </c>
-      <c r="E13" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1317,12 +1257,6 @@
       <c r="C14" t="s">
         <v>87</v>
       </c>
-      <c r="D14" t="s">
-        <v>175</v>
-      </c>
-      <c r="E14" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1334,12 +1268,6 @@
       <c r="C15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E15" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1351,14 +1279,8 @@
       <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
-        <v>175</v>
-      </c>
-      <c r="E16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
@@ -1368,14 +1290,8 @@
       <c r="C17" t="s">
         <v>77</v>
       </c>
-      <c r="D17" t="s">
-        <v>175</v>
-      </c>
-      <c r="E17" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -1385,14 +1301,8 @@
       <c r="C18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
-        <v>175</v>
-      </c>
-      <c r="E18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1402,14 +1312,8 @@
       <c r="C19" t="s">
         <v>84</v>
       </c>
-      <c r="D19" t="s">
-        <v>175</v>
-      </c>
-      <c r="E19" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
@@ -1419,14 +1323,8 @@
       <c r="C20" t="s">
         <v>71</v>
       </c>
-      <c r="D20" t="s">
-        <v>175</v>
-      </c>
-      <c r="E20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1436,14 +1334,8 @@
       <c r="C21" t="s">
         <v>72</v>
       </c>
-      <c r="D21" t="s">
-        <v>175</v>
-      </c>
-      <c r="E21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -1453,14 +1345,8 @@
       <c r="C22" t="s">
         <v>73</v>
       </c>
-      <c r="D22" t="s">
-        <v>175</v>
-      </c>
-      <c r="E22" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1470,14 +1356,8 @@
       <c r="C23" t="s">
         <v>74</v>
       </c>
-      <c r="D23" t="s">
-        <v>175</v>
-      </c>
-      <c r="E23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -1487,14 +1367,8 @@
       <c r="C24" t="s">
         <v>75</v>
       </c>
-      <c r="D24" t="s">
-        <v>175</v>
-      </c>
-      <c r="E24" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1504,14 +1378,8 @@
       <c r="C25" t="s">
         <v>76</v>
       </c>
-      <c r="D25" t="s">
-        <v>175</v>
-      </c>
-      <c r="E25" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1521,14 +1389,8 @@
       <c r="C26" t="s">
         <v>78</v>
       </c>
-      <c r="D26" t="s">
-        <v>175</v>
-      </c>
-      <c r="E26" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -1538,14 +1400,8 @@
       <c r="C27" t="s">
         <v>79</v>
       </c>
-      <c r="D27" t="s">
-        <v>175</v>
-      </c>
-      <c r="E27" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1555,14 +1411,8 @@
       <c r="C28" t="s">
         <v>80</v>
       </c>
-      <c r="D28" t="s">
-        <v>175</v>
-      </c>
-      <c r="E28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
@@ -1572,14 +1422,8 @@
       <c r="C29" t="s">
         <v>81</v>
       </c>
-      <c r="D29" t="s">
-        <v>175</v>
-      </c>
-      <c r="E29" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>49</v>
       </c>
@@ -1589,14 +1433,8 @@
       <c r="C30" t="s">
         <v>82</v>
       </c>
-      <c r="D30" t="s">
-        <v>175</v>
-      </c>
-      <c r="E30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>105</v>
       </c>
@@ -1606,14 +1444,8 @@
       <c r="C31" t="s">
         <v>103</v>
       </c>
-      <c r="D31" t="s">
-        <v>175</v>
-      </c>
-      <c r="E31" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>106</v>
       </c>
@@ -1622,12 +1454,6 @@
       </c>
       <c r="C32" t="s">
         <v>104</v>
-      </c>
-      <c r="D32" t="s">
-        <v>175</v>
-      </c>
-      <c r="E32" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1640,12 +1466,6 @@
       <c r="C33" t="s">
         <v>123</v>
       </c>
-      <c r="D33" t="s">
-        <v>175</v>
-      </c>
-      <c r="E33" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
@@ -1657,12 +1477,6 @@
       <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="D34" t="s">
-        <v>175</v>
-      </c>
-      <c r="E34" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
@@ -1674,12 +1488,6 @@
       <c r="C35" t="s">
         <v>101</v>
       </c>
-      <c r="D35" t="s">
-        <v>175</v>
-      </c>
-      <c r="E35" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
@@ -1691,12 +1499,6 @@
       <c r="C36" t="s">
         <v>20</v>
       </c>
-      <c r="D36" t="s">
-        <v>175</v>
-      </c>
-      <c r="E36" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
@@ -1708,12 +1510,6 @@
       <c r="C37" t="s">
         <v>102</v>
       </c>
-      <c r="D37" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
@@ -1725,12 +1521,6 @@
       <c r="C38" t="s">
         <v>94</v>
       </c>
-      <c r="D38" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
@@ -1742,12 +1532,6 @@
       <c r="C39" t="s">
         <v>95</v>
       </c>
-      <c r="D39" t="s">
-        <v>175</v>
-      </c>
-      <c r="E39" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
@@ -1759,12 +1543,6 @@
       <c r="C40" t="s">
         <v>96</v>
       </c>
-      <c r="D40" t="s">
-        <v>175</v>
-      </c>
-      <c r="E40" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -1776,12 +1554,6 @@
       <c r="C41" t="s">
         <v>115</v>
       </c>
-      <c r="D41" t="s">
-        <v>175</v>
-      </c>
-      <c r="E41" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
@@ -1793,12 +1565,6 @@
       <c r="C42" t="s">
         <v>116</v>
       </c>
-      <c r="D42" t="s">
-        <v>175</v>
-      </c>
-      <c r="E42" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
@@ -1810,12 +1576,6 @@
       <c r="C43" t="s">
         <v>117</v>
       </c>
-      <c r="D43" t="s">
-        <v>175</v>
-      </c>
-      <c r="E43" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
@@ -1827,16 +1587,10 @@
       <c r="C44" t="s">
         <v>120</v>
       </c>
-      <c r="D44" t="s">
-        <v>175</v>
-      </c>
-      <c r="E44" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
         <v>127</v>
@@ -1853,7 +1607,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B46" t="s">
         <v>128</v>
@@ -1870,7 +1624,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B47" t="s">
         <v>129</v>
@@ -1879,15 +1633,15 @@
         <v>140</v>
       </c>
       <c r="D47" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E47" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
         <v>130</v>
@@ -1904,7 +1658,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B49" t="s">
         <v>131</v>
@@ -1913,15 +1667,15 @@
         <v>145</v>
       </c>
       <c r="D49" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E49" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
         <v>132</v>
@@ -1930,15 +1684,15 @@
         <v>144</v>
       </c>
       <c r="D50" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E50" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B51" t="s">
         <v>133</v>
@@ -1947,66 +1701,66 @@
         <v>146</v>
       </c>
       <c r="D51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>151</v>
+        <v>222</v>
       </c>
       <c r="D52" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="E52" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B53" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C53" t="s">
-        <v>150</v>
+        <v>223</v>
       </c>
       <c r="D53" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
       <c r="E53" t="s">
-        <v>175</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" t="s">
         <v>169</v>
       </c>
-      <c r="C54" t="s">
-        <v>170</v>
-      </c>
-      <c r="D54" t="s">
-        <v>171</v>
-      </c>
       <c r="E54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B55" t="s">
         <v>134</v>
@@ -2015,32 +1769,32 @@
         <v>147</v>
       </c>
       <c r="D55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E55" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B56" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" t="s">
         <v>188</v>
       </c>
-      <c r="B56" t="s">
-        <v>189</v>
-      </c>
-      <c r="C56" t="s">
-        <v>190</v>
-      </c>
-      <c r="D56" t="s">
-        <v>191</v>
-      </c>
       <c r="E56" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B57" t="s">
         <v>135</v>
@@ -2049,66 +1803,66 @@
         <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B58" t="s">
         <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B59" t="s">
         <v>137</v>
       </c>
       <c r="C59" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" t="s">
         <v>166</v>
       </c>
-      <c r="D59" t="s">
-        <v>168</v>
-      </c>
       <c r="E59" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B60" t="s">
         <v>138</v>
       </c>
       <c r="C60" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B61" t="s">
         <v>139</v>
@@ -2117,62 +1871,62 @@
         <v>149</v>
       </c>
       <c r="D61" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E61" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B62" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C62" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C63" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B64" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C64" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B65" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C66" t="s">
         <v>1</v>
@@ -2180,10 +1934,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B67" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C67" t="s">
         <v>0</v>
@@ -2191,68 +1945,79 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B68" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C68" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C70" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B71" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B72" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C72" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B73" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>220</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" t="s">
+        <v>227</v>
+      </c>
+      <c r="C74" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added welcome panel and game icon
</commit_message>
<xml_diff>
--- a/Assets/Resources/CSV/Translations.xlsx
+++ b/Assets/Resources/CSV/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdude\OneDrive\Pulpit\Unity\Konrad_Dudek-Praca_Magisterska\Assets\Resources\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040C2D19-F522-4CAA-AACA-45783EA69C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B22785E2-823E-4899-83B5-EC73664EBC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="20376" windowHeight="12216" xr2:uid="{8D4D4752-D6F4-4947-96F6-AEAAB4AF41A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="238">
   <si>
     <t>Polish</t>
   </si>
@@ -723,6 +723,33 @@
   </si>
   <si>
     <t>Register sucessful!</t>
+  </si>
+  <si>
+    <t>LOGINSUCESSFUL</t>
+  </si>
+  <si>
+    <t>Zalogowano pomyślnie!</t>
+  </si>
+  <si>
+    <t>Login Sucessful!</t>
+  </si>
+  <si>
+    <t>PASSWORDTOOSHORT</t>
+  </si>
+  <si>
+    <t>Hasło musi się składać co najmniej z 6 znaków</t>
+  </si>
+  <si>
+    <t>The password must consist of at least 6 characters</t>
+  </si>
+  <si>
+    <t>ACCOUNTNOTFOUND</t>
+  </si>
+  <si>
+    <t>Takie konto nie istnieje</t>
+  </si>
+  <si>
+    <t>Account does not exist</t>
   </si>
 </sst>
 </file>
@@ -1085,10 +1112,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42FA13F9-4EBF-46CA-BDCD-3827A8DF10DF}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="B61" zoomScale="115" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2020,6 +2047,39 @@
         <v>228</v>
       </c>
     </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B75" t="s">
+        <v>230</v>
+      </c>
+      <c r="C75" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="B76" t="s">
+        <v>233</v>
+      </c>
+      <c r="C76" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B77" t="s">
+        <v>236</v>
+      </c>
+      <c r="C77" t="s">
+        <v>237</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>